<commit_message>
update the template and JSON to account for the doubly-nested arrays
</commit_message>
<xml_diff>
--- a/backend/reports/P_StatusPortfolioRollup_template.xlsx
+++ b/backend/reports/P_StatusPortfolioRollup_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\robrien\work\gdx-agreements-tracker\backend\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C748185D-C3FE-446F-996F-0AC53DF88E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCFF231-002B-412C-AED6-F8C936C1AF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="2385" windowWidth="28800" windowHeight="11385" xr2:uid="{924F95A4-5C33-44BA-889B-B48D51570D5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{924F95A4-5C33-44BA-889B-B48D51570D5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -259,11 +259,8 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -274,14 +271,17 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,140 +675,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" s="7" customFormat="1" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:10" s="6" customFormat="1" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="7" customFormat="1" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:10" s="6" customFormat="1" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="4"/>
+      <c r="H17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>